<commit_message>
Added sizes to data
</commit_message>
<xml_diff>
--- a/sample data/Sample EU Supreme Products for the Week of September 15 2022 (Week 4 of FW22) - One Sheet.xlsx
+++ b/sample data/Sample EU Supreme Products for the Week of September 15 2022 (Week 4 of FW22) - One Sheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="378">
   <si>
     <t>Name</t>
   </si>
@@ -55,6 +55,9 @@
     <t>Colors</t>
   </si>
   <si>
+    <t>Sizes</t>
+  </si>
+  <si>
     <t>Backpack</t>
   </si>
   <si>
@@ -1118,6 +1121,33 @@
   </si>
   <si>
     <t>Red,White,Black</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">129 ,139 ,149 </t>
+  </si>
+  <si>
+    <t>54MM</t>
+  </si>
+  <si>
+    <t>8 1/2</t>
+  </si>
+  <si>
+    <t>8 1/8</t>
+  </si>
+  <si>
+    <t>Small,Medium,Large,XLarge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 ,32 ,34 ,36 ,38 </t>
+  </si>
+  <si>
+    <t>Small,Medium,Large,XLarge,XXL</t>
+  </si>
+  <si>
+    <t>S/M,M/L</t>
   </si>
 </sst>
 </file>
@@ -1475,13 +1505,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M71"/>
+  <dimension ref="A1:N71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1521,19 +1551,22 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2">
         <v>307053</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E2">
         <v>138</v>
@@ -1554,27 +1587,30 @@
         <v>53</v>
       </c>
       <c r="K2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="L2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="M2" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
+        <v>303</v>
+      </c>
+      <c r="N2" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <v>307009</v>
       </c>
       <c r="C3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E3">
         <v>128</v>
@@ -1595,27 +1631,30 @@
         <v>54</v>
       </c>
       <c r="K3" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="L3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="M3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
+        <v>304</v>
+      </c>
+      <c r="N3" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4">
         <v>307037</v>
       </c>
       <c r="C4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D4" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E4">
         <v>128</v>
@@ -1636,27 +1675,30 @@
         <v>55</v>
       </c>
       <c r="K4" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="L4" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="M4" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
+        <v>305</v>
+      </c>
+      <c r="N4" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5">
         <v>307049</v>
       </c>
       <c r="C5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E5">
         <v>46</v>
@@ -1677,27 +1719,30 @@
         <v>56</v>
       </c>
       <c r="K5" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="L5" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="M5" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
+        <v>306</v>
+      </c>
+      <c r="N5" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B6">
         <v>307022</v>
       </c>
       <c r="C6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E6">
         <v>42</v>
@@ -1718,27 +1763,30 @@
         <v>57</v>
       </c>
       <c r="K6" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="L6" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="M6" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
+        <v>307</v>
+      </c>
+      <c r="N6" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7">
         <v>307004</v>
       </c>
       <c r="C7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E7">
         <v>48</v>
@@ -1759,27 +1807,30 @@
         <v>58</v>
       </c>
       <c r="K7" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="L7" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="M7" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
+        <v>308</v>
+      </c>
+      <c r="N7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B8">
         <v>307023</v>
       </c>
       <c r="C8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D8" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E8">
         <v>64</v>
@@ -1800,27 +1851,30 @@
         <v>66</v>
       </c>
       <c r="K8" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="L8" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="M8" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
+        <v>309</v>
+      </c>
+      <c r="N8" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9">
         <v>307054</v>
       </c>
       <c r="C9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D9" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E9">
         <v>32</v>
@@ -1841,27 +1895,30 @@
         <v>67</v>
       </c>
       <c r="K9" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="L9" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="M9" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
+        <v>310</v>
+      </c>
+      <c r="N9" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B10">
         <v>307011</v>
       </c>
       <c r="C10" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D10" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E10">
         <v>58</v>
@@ -1882,27 +1939,30 @@
         <v>68</v>
       </c>
       <c r="K10" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="L10" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="M10" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
+        <v>311</v>
+      </c>
+      <c r="N10" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B11">
         <v>307039</v>
       </c>
       <c r="C11" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D11" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E11">
         <v>58</v>
@@ -1923,27 +1983,30 @@
         <v>69</v>
       </c>
       <c r="K11" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="L11" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="M11" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
+        <v>312</v>
+      </c>
+      <c r="N11" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B12">
         <v>307085</v>
       </c>
       <c r="C12" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D12" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E12">
         <v>138</v>
@@ -1964,27 +2027,30 @@
         <v>13</v>
       </c>
       <c r="K12" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="L12" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="M12" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
+        <v>313</v>
+      </c>
+      <c r="N12" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B13">
         <v>307070</v>
       </c>
       <c r="C13" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D13" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E13">
         <v>128</v>
@@ -2005,27 +2071,30 @@
         <v>14</v>
       </c>
       <c r="K13" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="L13" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="M13" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
+        <v>314</v>
+      </c>
+      <c r="N13" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B14">
         <v>306984</v>
       </c>
       <c r="C14" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D14" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E14">
         <v>110</v>
@@ -2046,24 +2115,27 @@
         <v>15</v>
       </c>
       <c r="K14" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="M14" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13">
+        <v>315</v>
+      </c>
+      <c r="N14" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B15">
         <v>307034</v>
       </c>
       <c r="C15" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D15" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E15">
         <v>110</v>
@@ -2084,27 +2156,30 @@
         <v>16</v>
       </c>
       <c r="K15" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="L15" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="M15" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
+        <v>316</v>
+      </c>
+      <c r="N15" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B16">
         <v>307090</v>
       </c>
       <c r="C16" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D16" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E16">
         <v>178</v>
@@ -2125,27 +2200,30 @@
         <v>3</v>
       </c>
       <c r="K16" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="L16" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="M16" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13">
+        <v>317</v>
+      </c>
+      <c r="N16" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B17">
         <v>307079</v>
       </c>
       <c r="C17" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D17" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E17">
         <v>128</v>
@@ -2166,27 +2244,30 @@
         <v>36</v>
       </c>
       <c r="K17" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="L17" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="M17" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13">
+        <v>318</v>
+      </c>
+      <c r="N17" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B18">
         <v>307074</v>
       </c>
       <c r="C18" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D18" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E18">
         <v>158</v>
@@ -2207,27 +2288,30 @@
         <v>37</v>
       </c>
       <c r="K18" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="L18" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="M18" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13">
+        <v>319</v>
+      </c>
+      <c r="N18" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B19">
         <v>307010</v>
       </c>
       <c r="C19" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D19" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E19">
         <v>158</v>
@@ -2248,27 +2332,30 @@
         <v>38</v>
       </c>
       <c r="K19" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="L19" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="M19" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13">
+        <v>320</v>
+      </c>
+      <c r="N19" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B20">
         <v>307056</v>
       </c>
       <c r="C20" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D20" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E20">
         <v>118</v>
@@ -2289,27 +2376,30 @@
         <v>39</v>
       </c>
       <c r="K20" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="L20" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="M20" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13">
+        <v>321</v>
+      </c>
+      <c r="N20" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B21">
         <v>307064</v>
       </c>
       <c r="C21" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D21" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E21">
         <v>148</v>
@@ -2330,27 +2420,30 @@
         <v>40</v>
       </c>
       <c r="K21" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="L21" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="M21" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13">
+        <v>322</v>
+      </c>
+      <c r="N21" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B22">
         <v>307031</v>
       </c>
       <c r="C22" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D22" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E22">
         <v>158</v>
@@ -2371,27 +2464,30 @@
         <v>41</v>
       </c>
       <c r="K22" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="L22" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="M22" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13">
+        <v>323</v>
+      </c>
+      <c r="N22" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B23">
         <v>307026</v>
       </c>
       <c r="C23" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D23" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E23">
         <v>148</v>
@@ -2412,27 +2508,30 @@
         <v>42</v>
       </c>
       <c r="K23" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="L23" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="M23" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13">
+        <v>324</v>
+      </c>
+      <c r="N23" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B24">
         <v>307006</v>
       </c>
       <c r="C24" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D24" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E24">
         <v>158</v>
@@ -2453,27 +2552,30 @@
         <v>43</v>
       </c>
       <c r="K24" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="L24" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="M24" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13">
+        <v>325</v>
+      </c>
+      <c r="N24" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
       <c r="A25" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B25">
         <v>307014</v>
       </c>
       <c r="C25" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D25" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E25">
         <v>168</v>
@@ -2494,27 +2596,30 @@
         <v>44</v>
       </c>
       <c r="K25" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="L25" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="M25" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13">
+        <v>326</v>
+      </c>
+      <c r="N25" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B26">
         <v>306998</v>
       </c>
       <c r="C26" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D26" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E26">
         <v>148</v>
@@ -2535,27 +2640,30 @@
         <v>45</v>
       </c>
       <c r="K26" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="L26" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="M26" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13">
+        <v>327</v>
+      </c>
+      <c r="N26" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B27">
         <v>307087</v>
       </c>
       <c r="C27" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D27" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E27">
         <v>118</v>
@@ -2576,27 +2684,30 @@
         <v>4</v>
       </c>
       <c r="K27" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="L27" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="M27" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13">
+        <v>328</v>
+      </c>
+      <c r="N27" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B28">
         <v>307016</v>
       </c>
       <c r="C28" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D28" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E28">
         <v>110</v>
@@ -2617,27 +2728,30 @@
         <v>46</v>
       </c>
       <c r="K28" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="L28" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="M28" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13">
+        <v>329</v>
+      </c>
+      <c r="N28" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B29">
         <v>307086</v>
       </c>
       <c r="C29" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D29" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E29">
         <v>98</v>
@@ -2658,27 +2772,30 @@
         <v>2</v>
       </c>
       <c r="K29" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="L29" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="M29" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13">
+        <v>330</v>
+      </c>
+      <c r="N29" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B30">
         <v>307082</v>
       </c>
       <c r="C30" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D30" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E30">
         <v>42</v>
@@ -2699,27 +2816,30 @@
         <v>6</v>
       </c>
       <c r="K30" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="L30" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="M30" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13">
+        <v>331</v>
+      </c>
+      <c r="N30" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B31">
         <v>307084</v>
       </c>
       <c r="C31" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D31" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E31">
         <v>138</v>
@@ -2740,27 +2860,30 @@
         <v>11</v>
       </c>
       <c r="K31" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="L31" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="M31" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13">
+        <v>332</v>
+      </c>
+      <c r="N31" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
       <c r="A32" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B32">
         <v>307092</v>
       </c>
       <c r="C32" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D32" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E32">
         <v>88</v>
@@ -2781,27 +2904,30 @@
         <v>24</v>
       </c>
       <c r="K32" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="L32" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="M32" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13">
+        <v>333</v>
+      </c>
+      <c r="N32" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
       <c r="A33" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B33">
         <v>307080</v>
       </c>
       <c r="C33" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D33" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E33">
         <v>78</v>
@@ -2822,27 +2948,30 @@
         <v>25</v>
       </c>
       <c r="K33" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="L33" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="M33" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13">
+        <v>334</v>
+      </c>
+      <c r="N33" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
       <c r="A34" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B34">
         <v>307018</v>
       </c>
       <c r="C34" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D34" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E34">
         <v>178</v>
@@ -2863,27 +2992,30 @@
         <v>12</v>
       </c>
       <c r="K34" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="L34" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="M34" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13">
+        <v>335</v>
+      </c>
+      <c r="N34" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
       <c r="A35" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B35">
         <v>307060</v>
       </c>
       <c r="C35" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D35" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E35">
         <v>118</v>
@@ -2904,27 +3036,30 @@
         <v>26</v>
       </c>
       <c r="K35" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="L35" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="M35" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13">
+        <v>336</v>
+      </c>
+      <c r="N35" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
       <c r="A36" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B36">
         <v>306999</v>
       </c>
       <c r="C36" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D36" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E36">
         <v>68</v>
@@ -2945,27 +3080,30 @@
         <v>27</v>
       </c>
       <c r="K36" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="L36" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="M36" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13">
+        <v>337</v>
+      </c>
+      <c r="N36" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
       <c r="A37" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B37">
         <v>307059</v>
       </c>
       <c r="C37" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D37" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E37">
         <v>88</v>
@@ -2986,27 +3124,30 @@
         <v>28</v>
       </c>
       <c r="K37" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="L37" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="M37" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13">
+        <v>338</v>
+      </c>
+      <c r="N37" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
       <c r="A38" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B38">
         <v>307015</v>
       </c>
       <c r="C38" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D38" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E38">
         <v>52</v>
@@ -3027,27 +3168,30 @@
         <v>29</v>
       </c>
       <c r="K38" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="L38" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="M38" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13">
+        <v>339</v>
+      </c>
+      <c r="N38" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
       <c r="A39" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B39">
         <v>307062</v>
       </c>
       <c r="C39" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D39" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E39">
         <v>78</v>
@@ -3068,27 +3212,30 @@
         <v>30</v>
       </c>
       <c r="K39" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="L39" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="M39" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13">
+        <v>340</v>
+      </c>
+      <c r="N39" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
       <c r="A40" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B40">
         <v>307051</v>
       </c>
       <c r="C40" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D40" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E40">
         <v>40</v>
@@ -3109,27 +3256,30 @@
         <v>31</v>
       </c>
       <c r="K40" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L40" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="M40" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13">
+        <v>341</v>
+      </c>
+      <c r="N40" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
       <c r="A41" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B41">
         <v>307050</v>
       </c>
       <c r="C41" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D41" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E41">
         <v>40</v>
@@ -3150,27 +3300,30 @@
         <v>32</v>
       </c>
       <c r="K41" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L41" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="M41" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13">
+        <v>342</v>
+      </c>
+      <c r="N41" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
       <c r="A42" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B42">
         <v>306985</v>
       </c>
       <c r="C42" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D42" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E42">
         <v>40</v>
@@ -3191,27 +3344,30 @@
         <v>33</v>
       </c>
       <c r="K42" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L42" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="M42" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13">
+        <v>343</v>
+      </c>
+      <c r="N42" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
       <c r="A43" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B43">
         <v>306996</v>
       </c>
       <c r="C43" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D43" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E43">
         <v>40</v>
@@ -3232,27 +3388,30 @@
         <v>34</v>
       </c>
       <c r="K43" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L43" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="M43" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13">
+        <v>344</v>
+      </c>
+      <c r="N43" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14">
       <c r="A44" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B44">
         <v>307044</v>
       </c>
       <c r="C44" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D44" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E44">
         <v>40</v>
@@ -3273,27 +3432,30 @@
         <v>35</v>
       </c>
       <c r="K44" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L44" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="M44" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13">
+        <v>345</v>
+      </c>
+      <c r="N44" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14">
       <c r="A45" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B45">
         <v>307081</v>
       </c>
       <c r="C45" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D45" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E45">
         <v>288</v>
@@ -3314,27 +3476,30 @@
         <v>0</v>
       </c>
       <c r="K45" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="L45" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="M45" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13">
+        <v>346</v>
+      </c>
+      <c r="N45" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14">
       <c r="A46" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B46">
         <v>307076</v>
       </c>
       <c r="C46" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D46" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E46">
         <v>208</v>
@@ -3355,27 +3520,30 @@
         <v>1</v>
       </c>
       <c r="K46" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="L46" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="M46" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13">
+        <v>347</v>
+      </c>
+      <c r="N46" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14">
       <c r="A47" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B47">
         <v>307042</v>
       </c>
       <c r="C47" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D47" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E47">
         <v>178</v>
@@ -3396,27 +3564,30 @@
         <v>7</v>
       </c>
       <c r="K47" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="L47" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="M47" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13">
+        <v>348</v>
+      </c>
+      <c r="N47" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14">
       <c r="A48" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B48">
         <v>307068</v>
       </c>
       <c r="C48" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D48" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E48">
         <v>178</v>
@@ -3437,27 +3608,30 @@
         <v>8</v>
       </c>
       <c r="K48" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="L48" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="M48" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13">
+        <v>349</v>
+      </c>
+      <c r="N48" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14">
       <c r="A49" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B49">
         <v>306997</v>
       </c>
       <c r="C49" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D49" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E49">
         <v>428</v>
@@ -3478,27 +3652,30 @@
         <v>9</v>
       </c>
       <c r="K49" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="L49" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="M49" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13">
+        <v>350</v>
+      </c>
+      <c r="N49" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14">
       <c r="A50" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B50">
         <v>307067</v>
       </c>
       <c r="C50" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D50" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E50">
         <v>128</v>
@@ -3519,27 +3696,30 @@
         <v>10</v>
       </c>
       <c r="K50" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="L50" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="M50" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13">
+        <v>351</v>
+      </c>
+      <c r="N50" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14">
       <c r="A51" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B51">
         <v>307077</v>
       </c>
       <c r="C51" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D51" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E51">
         <v>178</v>
@@ -3560,27 +3740,30 @@
         <v>17</v>
       </c>
       <c r="K51" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="L51" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="M51" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13">
+        <v>352</v>
+      </c>
+      <c r="N51" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14">
       <c r="A52" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B52">
         <v>307078</v>
       </c>
       <c r="C52" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D52" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E52">
         <v>148</v>
@@ -3601,27 +3784,30 @@
         <v>18</v>
       </c>
       <c r="K52" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="L52" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="M52" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13">
+        <v>353</v>
+      </c>
+      <c r="N52" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14">
       <c r="A53" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B53">
         <v>306989</v>
       </c>
       <c r="C53" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D53" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E53">
         <v>168</v>
@@ -3642,27 +3828,30 @@
         <v>19</v>
       </c>
       <c r="K53" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="L53" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="M53" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13">
+        <v>354</v>
+      </c>
+      <c r="N53" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14">
       <c r="A54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B54">
         <v>307073</v>
       </c>
       <c r="C54" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D54" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E54">
         <v>148</v>
@@ -3683,27 +3872,30 @@
         <v>20</v>
       </c>
       <c r="K54" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="L54" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="M54" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13">
+        <v>355</v>
+      </c>
+      <c r="N54" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14">
       <c r="A55" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B55">
         <v>307030</v>
       </c>
       <c r="C55" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D55" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E55">
         <v>128</v>
@@ -3724,27 +3916,30 @@
         <v>21</v>
       </c>
       <c r="K55" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="L55" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="M55" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13">
+        <v>356</v>
+      </c>
+      <c r="N55" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14">
       <c r="A56" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B56">
         <v>307005</v>
       </c>
       <c r="C56" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D56" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E56">
         <v>148</v>
@@ -3765,27 +3960,30 @@
         <v>22</v>
       </c>
       <c r="K56" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="L56" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="M56" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13">
+        <v>357</v>
+      </c>
+      <c r="N56" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14">
       <c r="A57" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B57">
         <v>307071</v>
       </c>
       <c r="C57" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D57" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E57">
         <v>168</v>
@@ -3806,27 +4004,30 @@
         <v>23</v>
       </c>
       <c r="K57" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="L57" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="M57" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13">
+        <v>358</v>
+      </c>
+      <c r="N57" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14">
       <c r="A58" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B58">
         <v>307083</v>
       </c>
       <c r="C58" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D58" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E58">
         <v>42</v>
@@ -3847,27 +4048,30 @@
         <v>5</v>
       </c>
       <c r="K58" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="L58" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="M58" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13">
+        <v>346</v>
+      </c>
+      <c r="N58" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14">
       <c r="A59" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B59">
         <v>307089</v>
       </c>
       <c r="C59" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D59" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E59">
         <v>46</v>
@@ -3888,27 +4092,30 @@
         <v>47</v>
       </c>
       <c r="K59" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="L59" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="M59" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13">
+        <v>359</v>
+      </c>
+      <c r="N59" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14">
       <c r="A60" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B60">
         <v>307088</v>
       </c>
       <c r="C60" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D60" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E60">
         <v>50</v>
@@ -3929,27 +4136,30 @@
         <v>48</v>
       </c>
       <c r="K60" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="L60" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="M60" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13">
+        <v>360</v>
+      </c>
+      <c r="N60" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14">
       <c r="A61" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B61">
         <v>307000</v>
       </c>
       <c r="C61" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D61" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E61">
         <v>46</v>
@@ -3970,27 +4180,30 @@
         <v>49</v>
       </c>
       <c r="K61" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="L61" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="M61" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13">
+        <v>361</v>
+      </c>
+      <c r="N61" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14">
       <c r="A62" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B62">
         <v>307075</v>
       </c>
       <c r="C62" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D62" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E62">
         <v>54</v>
@@ -4011,27 +4224,30 @@
         <v>50</v>
       </c>
       <c r="K62" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="L62" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="M62" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13">
+        <v>362</v>
+      </c>
+      <c r="N62" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14">
       <c r="A63" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B63">
         <v>306986</v>
       </c>
       <c r="C63" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D63" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E63">
         <v>44</v>
@@ -4052,27 +4268,30 @@
         <v>51</v>
       </c>
       <c r="K63" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="L63" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="M63" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13">
+        <v>363</v>
+      </c>
+      <c r="N63" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14">
       <c r="A64" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B64">
         <v>306981</v>
       </c>
       <c r="C64" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D64" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E64">
         <v>34</v>
@@ -4093,27 +4312,30 @@
         <v>52</v>
       </c>
       <c r="K64" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="L64" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="M64" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13">
+        <v>364</v>
+      </c>
+      <c r="N64" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14">
       <c r="A65" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B65">
         <v>307091</v>
       </c>
       <c r="C65" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D65" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E65">
         <v>88</v>
@@ -4134,27 +4356,30 @@
         <v>59</v>
       </c>
       <c r="K65" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L65" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="M65" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13">
+        <v>352</v>
+      </c>
+      <c r="N65" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14">
       <c r="A66" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B66">
         <v>307002</v>
       </c>
       <c r="C66" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D66" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E66">
         <v>48</v>
@@ -4175,27 +4400,30 @@
         <v>60</v>
       </c>
       <c r="K66" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L66" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="M66" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="67" spans="1:13">
+        <v>365</v>
+      </c>
+      <c r="N66" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14">
       <c r="A67" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B67">
         <v>307007</v>
       </c>
       <c r="C67" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D67" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E67">
         <v>28</v>
@@ -4216,27 +4444,30 @@
         <v>61</v>
       </c>
       <c r="K67" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L67" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="M67" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13">
+        <v>366</v>
+      </c>
+      <c r="N67" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14">
       <c r="A68" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B68">
         <v>306994</v>
       </c>
       <c r="C68" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D68" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E68">
         <v>30</v>
@@ -4257,27 +4488,30 @@
         <v>62</v>
       </c>
       <c r="K68" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L68" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="M68" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13">
+        <v>367</v>
+      </c>
+      <c r="N68" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14">
       <c r="A69" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B69">
         <v>307041</v>
       </c>
       <c r="C69" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D69" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E69">
         <v>36</v>
@@ -4298,27 +4532,30 @@
         <v>63</v>
       </c>
       <c r="K69" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L69" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="M69" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13">
+        <v>366</v>
+      </c>
+      <c r="N69" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14">
       <c r="A70" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B70">
         <v>307043</v>
       </c>
       <c r="C70" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D70" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E70">
         <v>28</v>
@@ -4339,27 +4576,30 @@
         <v>64</v>
       </c>
       <c r="K70" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L70" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="M70" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13">
+        <v>368</v>
+      </c>
+      <c r="N70" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14">
       <c r="A71" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B71">
         <v>307046</v>
       </c>
       <c r="C71" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D71" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E71">
         <v>20</v>
@@ -4380,13 +4620,16 @@
         <v>65</v>
       </c>
       <c r="K71" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L71" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="M71" t="s">
-        <v>365</v>
+        <v>366</v>
+      </c>
+      <c r="N71" t="s">
+        <v>369</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added stock levels to data
</commit_message>
<xml_diff>
--- a/sample data/Sample EU Supreme Products for the Week of September 15 2022 (Week 4 of FW22) - One Sheet.xlsx
+++ b/sample data/Sample EU Supreme Products for the Week of September 15 2022 (Week 4 of FW22) - One Sheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="448">
   <si>
     <t>Name</t>
   </si>
@@ -58,6 +58,9 @@
     <t>Sizes</t>
   </si>
   <si>
+    <t>Stock Levels</t>
+  </si>
+  <si>
     <t>Backpack</t>
   </si>
   <si>
@@ -1148,6 +1151,213 @@
   </si>
   <si>
     <t>S/M,M/L</t>
+  </si>
+  <si>
+    <t>0, 'END OF STOCK FOR Silver', 0, 'END OF STOCK FOR Red', 1, 'END OF STOCK FOR Olive', 0, 'END OF STOCK FOR Black'</t>
+  </si>
+  <si>
+    <t>0, 'END OF STOCK FOR Red', 0, 'END OF STOCK FOR Silver', 1, 'END OF STOCK FOR Black', 1, 'END OF STOCK FOR Olive'</t>
+  </si>
+  <si>
+    <t>0, 'END OF STOCK FOR Black', 0, 'END OF STOCK FOR Red', 0, 'END OF STOCK FOR Olive', 0, 'END OF STOCK FOR Silver'</t>
+  </si>
+  <si>
+    <t>0, 'END OF STOCK FOR Olive', 0, 'END OF STOCK FOR Silver', 0, 'END OF STOCK FOR Black', 0, 'END OF STOCK FOR Red'</t>
+  </si>
+  <si>
+    <t>0, 'END OF STOCK FOR Silver', 0, 'END OF STOCK FOR Black', 0, 'END OF STOCK FOR Olive', 0, 'END OF STOCK FOR Red'</t>
+  </si>
+  <si>
+    <t>1, 'END OF STOCK FOR Black', 0, 'END OF STOCK FOR Red', 1, 'END OF STOCK FOR Silver', 1, 'END OF STOCK FOR Olive'</t>
+  </si>
+  <si>
+    <t>1, 1, 1, 'END OF STOCK FOR Silver'</t>
+  </si>
+  <si>
+    <t>1, 'END OF STOCK FOR Swirl 54mm', 1, 'END OF STOCK FOR White 52mm'</t>
+  </si>
+  <si>
+    <t>1, 'END OF STOCK FOR White - 8.5" x 32"'</t>
+  </si>
+  <si>
+    <t>1, 'END OF STOCK FOR Green - 8.125" x 32" ', 1, 'END OF STOCK FOR Black - 8.25" x 32" ', 1, 'END OF STOCK FOR White - 8" x 31.875" '</t>
+  </si>
+  <si>
+    <t>1, 1, 1, 0, 'END OF STOCK FOR Dark Plum', 1, 1, 1, 1, 'END OF STOCK FOR Black', 1, 1, 1, 1, 'END OF STOCK FOR Gold'</t>
+  </si>
+  <si>
+    <t>1, 1, 1, 0, 'END OF STOCK FOR Black', 1, 1, 1, 1, 'END OF STOCK FOR Light Brown'</t>
+  </si>
+  <si>
+    <t>0, 0, 0, 0, 'END OF STOCK FOR Denim', 1, 1, 1, 1, 'END OF STOCK FOR Red', 0, 0, 1, 0, 'END OF STOCK FOR Grey', 1, 1, 1, 0, 'END OF STOCK FOR Purple', 0, 0, 0, 0, 'END OF STOCK FOR Olive', 0, 0, 0, 0, 'END OF STOCK FOR Natural', 1, 1, 1, 1, 'END OF STOCK FOR Black'</t>
+  </si>
+  <si>
+    <t>0, 1, 1, 0, 'END OF STOCK FOR Pink', 1, 1, 1, 0, 'END OF STOCK FOR Black', 0, 1, 1, 1, 'END OF STOCK FOR Rust'</t>
+  </si>
+  <si>
+    <t>0, 0, 0, 0, 'END OF STOCK FOR Washed Blue', 0, 0, 0, 0, 'END OF STOCK FOR Gold Snakeskin', 0, 0, 0, 0, 'END OF STOCK FOR Black'</t>
+  </si>
+  <si>
+    <t>0, 1, 1, 1, 0, 'END OF STOCK FOR Burnt Orange', 1, 1, 1, 0, 0, 'END OF STOCK FOR Black', 1, 0, 1, 1, 1, 'END OF STOCK FOR Olive', 1, 1, 1, 1, 0, 'END OF STOCK FOR Slate', 1, 1, 1, 1, 0, 'END OF STOCK FOR Brown'</t>
+  </si>
+  <si>
+    <t>0, 0, 1, 1, 0, 'END OF STOCK FOR Reverse Indigo', 1, 1, 0, 1, 0, 'END OF STOCK FOR Brown'</t>
+  </si>
+  <si>
+    <t>0, 0, 0, 0, 0, 'END OF STOCK FOR Brown', 0, 0, 0, 0, 0, 'END OF STOCK FOR Red', 0, 0, 0, 0, 0, 'END OF STOCK FOR Black'</t>
+  </si>
+  <si>
+    <t>0, 0, 0, 0, 0, 'END OF STOCK FOR Burgundy', 0, 0, 0, 0, 0, 'END OF STOCK FOR Olive', 0, 0, 0, 0, 0, 'END OF STOCK FOR Black'</t>
+  </si>
+  <si>
+    <t>1, 1, 1, 0, 0, 'END OF STOCK FOR Branch Woodland Camo', 0, 0, 0, 0, 0, 'END OF STOCK FOR Black', 0, 0, 0, 0, 0, 'END OF STOCK FOR White', 0, 0, 0, 0, 0, 'END OF STOCK FOR Brown'</t>
+  </si>
+  <si>
+    <t>1, 1, 1, 0, 0, 'END OF STOCK FOR Heather Grey', 1, 0, 1, 0, 0, 'END OF STOCK FOR Black', 1, 1, 1, 0, 0, 'END OF STOCK FOR Green'</t>
+  </si>
+  <si>
+    <t>1, 0, 1, 0, 0, 'END OF STOCK FOR Dyed Rust', 1, 1, 1, 1, 1, 'END OF STOCK FOR Washed Blue', 1, 1, 1, 1, 1, 'END OF STOCK FOR Washed Black', 0, 0, 0, 0, 0, 'END OF STOCK FOR Natural'</t>
+  </si>
+  <si>
+    <t>1, 1, 1, 1, 0, 'END OF STOCK FOR Rigid Indigo'</t>
+  </si>
+  <si>
+    <t>1, 1, 1, 1, 0, 'END OF STOCK FOR Stone Washed Indigo'</t>
+  </si>
+  <si>
+    <t>1, 1, 1, 1, 1, 'END OF STOCK FOR Washed Black'</t>
+  </si>
+  <si>
+    <t>0, 0, 0, 0, 'END OF STOCK FOR Black', 0, 0, 0, 0, 'END OF STOCK FOR Gold Snakeskin', 0, 0, 0, 0, 'END OF STOCK FOR Mint Snakeskin'</t>
+  </si>
+  <si>
+    <t>1, 1, 1, 0, 0, 'END OF STOCK FOR Ash Grey', 1, 1, 1, 1, 1, 'END OF STOCK FOR Light Olive', 1, 1, 1, 1, 0, 'END OF STOCK FOR Bright Orange', 1, 1, 1, 1, 1, 'END OF STOCK FOR Raspberry', 1, 1, 1, 1, 0, 'END OF STOCK FOR Dark Brown', 1, 1, 1, 1, 0, 'END OF STOCK FOR Light Slate', 1, 1, 1, 1, 1, 'END OF STOCK FOR Black'</t>
+  </si>
+  <si>
+    <t>0, 0, 0, 0, 'END OF STOCK FOR Pale Green', 0, 0, 0, 0, 'END OF STOCK FOR Black', 0, 0, 0, 0, 'END OF STOCK FOR Dusty Blue'</t>
+  </si>
+  <si>
+    <t>0, 0, 0, 0, 'END OF STOCK FOR Orange', 0, 0, 0, 0, 'END OF STOCK FOR White', 1, 1, 1, 1, 'END OF STOCK FOR Green', 0, 0, 0, 0, 'END OF STOCK FOR Black', 0, 1, 0, 0, 'END OF STOCK FOR Blue'</t>
+  </si>
+  <si>
+    <t>1, 1, 1, 1, 'END OF STOCK FOR Multicolor', 0, 0, 1, 0, 'END OF STOCK FOR Black'</t>
+  </si>
+  <si>
+    <t>0, 1, 1, 1, 1, 'END OF STOCK FOR Washed Navy', 1, 1, 1, 1, 1, 'END OF STOCK FOR Olive', 1, 1, 1, 1, 1, 'END OF STOCK FOR Black', 1, 1, 1, 1, 0, 'END OF STOCK FOR Pale Pink'</t>
+  </si>
+  <si>
+    <t>1, 1, 1, 1, 1, 'END OF STOCK FOR Neon Green', 1, 1, 1, 1, 1, 'END OF STOCK FOR Grey', 1, 1, 1, 1, 1, 'END OF STOCK FOR Red', 1, 1, 1, 1, 1, 'END OF STOCK FOR White'</t>
+  </si>
+  <si>
+    <t>1, 0, 0, 0, 'END OF STOCK FOR Olive', 1, 1, 1, 1, 'END OF STOCK FOR Black', 1, 0, 1, 1, 'END OF STOCK FOR Plum', 1, 1, 1, 1, 'END OF STOCK FOR Light Brown'</t>
+  </si>
+  <si>
+    <t>0, 0, 1, 1, 0, 'END OF STOCK FOR Black', 0, 0, 0, 0, 0, 'END OF STOCK FOR White', 0, 1, 1, 1, 0, 'END OF STOCK FOR Brown'</t>
+  </si>
+  <si>
+    <t>0, 1, 1, 1, 0, 'END OF STOCK FOR Bright Pink', 1, 1, 1, 1, 1, 'END OF STOCK FOR White', 1, 1, 1, 1, 0, 'END OF STOCK FOR Dark Green', 1, 1, 1, 1, 1, 'END OF STOCK FOR Black', 1, 1, 1, 1, 1, 'END OF STOCK FOR Dark Tan', 0, 1, 1, 1, 0, 'END OF STOCK FOR Dark Navy'</t>
+  </si>
+  <si>
+    <t>1, 1, 1, 1, 0, 'END OF STOCK FOR Green', 1, 1, 1, 1, 1, 'END OF STOCK FOR Black'</t>
+  </si>
+  <si>
+    <t>0, 1, 1, 1, 0, 'END OF STOCK FOR Navy', 1, 1, 1, 1, 1, 'END OF STOCK FOR Branch Woodland Camo', 0, 1, 1, 1, 0, 'END OF STOCK FOR Ash Grey', 0, 1, 1, 1, 0, 'END OF STOCK FOR Black', 1, 1, 1, 1, 0, 'END OF STOCK FOR Magenta', 0, 1, 1, 1, 0, 'END OF STOCK FOR White', 1, 1, 1, 1, 0, 'END OF STOCK FOR Brown', 1, 1, 1, 1, 0, 'END OF STOCK FOR Teal'</t>
+  </si>
+  <si>
+    <t>0, 0, 0, 1, 0, 'END OF STOCK FOR Dusty Yellow', 0, 1, 1, 1, 1, 'END OF STOCK FOR Black', 0, 1, 1, 1, 1, 'END OF STOCK FOR White', 0, 1, 1, 1, 0, 'END OF STOCK FOR Dark Olive', 0, 1, 1, 1, 1, 'END OF STOCK FOR Red', 0, 1, 1, 1, 1, 'END OF STOCK FOR Teal'</t>
+  </si>
+  <si>
+    <t>1, 1, 1, 0, 0, 'END OF STOCK FOR Black', 1, 1, 1, 1, 0, 'END OF STOCK FOR Eggplant', 1, 1, 1, 1, 0, 'END OF STOCK FOR Heather Grey', 1, 1, 1, 1, 0, 'END OF STOCK FOR Orange', 1, 1, 1, 1, 0, 'END OF STOCK FOR White', 1, 1, 1, 1, 0, 'END OF STOCK FOR Light Olive'</t>
+  </si>
+  <si>
+    <t>0, 0, 0, 0, 0, 'END OF STOCK FOR Purple', 0, 1, 1, 1, 0, 'END OF STOCK FOR White', 0, 1, 1, 1, 0, 'END OF STOCK FOR Green', 0, 1, 1, 0, 0, 'END OF STOCK FOR Red', 0, 1, 1, 1, 0, 'END OF STOCK FOR Black', 0, 1, 1, 1, 0, 'END OF STOCK FOR Brown'</t>
+  </si>
+  <si>
+    <t>1, 1, 1, 1, 0, 'END OF STOCK FOR Black', 1, 1, 1, 1, 0, 'END OF STOCK FOR Green', 1, 1, 1, 1, 0, 'END OF STOCK FOR Brown', 0, 1, 1, 1, 1, 'END OF STOCK FOR Light Pink', 1, 1, 1, 1, 1, 'END OF STOCK FOR Eggplant', 1, 1, 1, 1, 1, 'END OF STOCK FOR White'</t>
+  </si>
+  <si>
+    <t>1, 1, 1, 1, 1, 'END OF STOCK FOR Green', 1, 1, 1, 1, 1, 'END OF STOCK FOR White', 1, 1, 1, 1, 0, 'END OF STOCK FOR Brown', 1, 1, 1, 1, 1, 'END OF STOCK FOR Magenta', 1, 1, 1, 1, 0, 'END OF STOCK FOR Black', 1, 1, 1, 1, 1, 'END OF STOCK FOR Heather Grey'</t>
+  </si>
+  <si>
+    <t>1, 1, 1, 1, 0, 'END OF STOCK FOR Black', 1, 1, 1, 1, 0, 'END OF STOCK FOR Dusty Blue', 1, 1, 1, 1, 0, 'END OF STOCK FOR Brown', 1, 1, 1, 1, 1, 'END OF STOCK FOR Light Pink', 1, 1, 1, 1, 1, 'END OF STOCK FOR White'</t>
+  </si>
+  <si>
+    <t>0, 0, 0, 0, 'END OF STOCK FOR Gold Snakeskin', 0, 0, 0, 0, 'END OF STOCK FOR Washed Blue', 0, 0, 0, 0, 'END OF STOCK FOR Black'</t>
+  </si>
+  <si>
+    <t>0, 0, 0, 0, 'END OF STOCK FOR Mint Snakeskin', 0, 0, 0, 0, 'END OF STOCK FOR Black', 0, 0, 0, 0, 'END OF STOCK FOR Gold Snakeskin'</t>
+  </si>
+  <si>
+    <t>0, 1, 1, 1, 0, 'END OF STOCK FOR Black', 0, 0, 1, 1, 0, 'END OF STOCK FOR Red', 1, 0, 0, 1, 0, 'END OF STOCK FOR Brown'</t>
+  </si>
+  <si>
+    <t>1, 1, 1, 1, 'END OF STOCK FOR Sulfur', 1, 1, 1, 0, 'END OF STOCK FOR Black', 1, 1, 1, 0, 'END OF STOCK FOR Dusty Lilac'</t>
+  </si>
+  <si>
+    <t>0, 1, 1, 0, 'END OF STOCK FOR Desert Camo', 1, 1, 1, 1, 'END OF STOCK FOR Black', 1, 1, 1, 1, 'END OF STOCK FOR Yellow'</t>
+  </si>
+  <si>
+    <t>0, 0, 0, 0, 0, 'END OF STOCK FOR Burgundy', 0, 0, 0, 0, 0, 'END OF STOCK FOR Black', 0, 0, 0, 0, 0, 'END OF STOCK FOR Olive'</t>
+  </si>
+  <si>
+    <t>1, 1, 1, 1, 1, 'END OF STOCK FOR Multicolor'</t>
+  </si>
+  <si>
+    <t>1, 1, 1, 1, 1, 'END OF STOCK FOR Heather Grey', 0, 1, 1, 1, 0, 'END OF STOCK FOR Washed Royal', 1, 1, 1, 1, 1, 'END OF STOCK FOR Bright Orange', 1, 1, 1, 1, 1, 'END OF STOCK FOR White', 1, 1, 1, 1, 1, 'END OF STOCK FOR Pale Yellow', 1, 1, 1, 1, 1, 'END OF STOCK FOR Black', 1, 1, 1, 1, 1, 'END OF STOCK FOR Light Olive'</t>
+  </si>
+  <si>
+    <t>1, 1, 1, 1, 1, 'END OF STOCK FOR Black', 1, 1, 1, 1, 0, 'END OF STOCK FOR Green', 1, 1, 1, 1, 1, 'END OF STOCK FOR Heather Grey'</t>
+  </si>
+  <si>
+    <t>1, 0, 1, 0, 0, 'END OF STOCK FOR Bright Gold', 1, 1, 1, 1, 1, 'END OF STOCK FOR Dark Brown', 0, 1, 1, 1, 0, 'END OF STOCK FOR Red', 0, 0, 0, 0, 0, 'END OF STOCK FOR Navy', 1, 1, 1, 1, 1, 'END OF STOCK FOR Ash Grey', 1, 1, 1, 1, 1, 'END OF STOCK FOR Black', 1, 1, 1, 1, 0, 'END OF STOCK FOR Dark Aqua'</t>
+  </si>
+  <si>
+    <t>0, 1, 1, 1, 0, 'END OF STOCK FOR Black', 1, 1, 1, 1, 1, 'END OF STOCK FOR Raspberry', 0, 0, 1, 1, 0, 'END OF STOCK FOR Ash Grey', 1, 1, 1, 1, 1, 'END OF STOCK FOR Dark Brown', 1, 1, 1, 1, 0, 'END OF STOCK FOR Light Olive', 0, 1, 1, 1, 1, 'END OF STOCK FOR Light Slate', 1, 1, 1, 1, 0, 'END OF STOCK FOR Bright Orange'</t>
+  </si>
+  <si>
+    <t>1, 1, 1, 1, 1, 'END OF STOCK FOR Ash Grey', 1, 1, 1, 1, 1, 'END OF STOCK FOR Burgundy', 1, 1, 1, 1, 1, 'END OF STOCK FOR Woodland Camo', 1, 1, 1, 1, 1, 'END OF STOCK FOR Black', 0, 0, 0, 1, 0, 'END OF STOCK FOR Purple'</t>
+  </si>
+  <si>
+    <t>1, 1, 1, 1, 0, 'END OF STOCK FOR Brown', 1, 1, 1, 1, 1, 'END OF STOCK FOR Ash Grey', 1, 1, 1, 0, 0, 'END OF STOCK FOR Royal', 1, 1, 1, 1, 1, 'END OF STOCK FOR Black'</t>
+  </si>
+  <si>
+    <t>0, 'END OF STOCK FOR Gold Snakeskin', 0, 'END OF STOCK FOR Washed Blue', 0, 'END OF STOCK FOR Black'</t>
+  </si>
+  <si>
+    <t>1, 'END OF STOCK FOR Branch Olive Camo', 1, 'END OF STOCK FOR Yellow', 1, 'END OF STOCK FOR Black', 1, 'END OF STOCK FOR Brown', 1, 'END OF STOCK FOR Light Blue'</t>
+  </si>
+  <si>
+    <t>1, 'END OF STOCK FOR Black', 1, 'END OF STOCK FOR Khaki', 1, 'END OF STOCK FOR Red', 1, 'END OF STOCK FOR Teal'</t>
+  </si>
+  <si>
+    <t>1, 'END OF STOCK FOR Green', 0, 'END OF STOCK FOR Black', 0, 'END OF STOCK FOR Red', 0, 'END OF STOCK FOR Brown', 0, 'END OF STOCK FOR Navy', 1, 'END OF STOCK FOR White'</t>
+  </si>
+  <si>
+    <t>1, 1, 'END OF STOCK FOR Red', 1, 1, 'END OF STOCK FOR Pale Blue', 1, 1, 'END OF STOCK FOR Olive', 1, 1, 'END OF STOCK FOR Stone', 1, 1, 'END OF STOCK FOR Black'</t>
+  </si>
+  <si>
+    <t>1, 'END OF STOCK FOR Navy', 1, 'END OF STOCK FOR Brown', 1, 'END OF STOCK FOR Green', 1, 'END OF STOCK FOR Grey', 1, 'END OF STOCK FOR Black', 1, 'END OF STOCK FOR Light Blue'</t>
+  </si>
+  <si>
+    <t>1, 'END OF STOCK FOR Brown', 1, 'END OF STOCK FOR Yellow', 1, 'END OF STOCK FOR Light Blue', 1, 'END OF STOCK FOR Black', 1, 'END OF STOCK FOR Olive'</t>
+  </si>
+  <si>
+    <t>1, 'END OF STOCK FOR Multicolor'</t>
+  </si>
+  <si>
+    <t>1, 'END OF STOCK FOR Black', 1, 'END OF STOCK FOR Red'</t>
+  </si>
+  <si>
+    <t>1, 1, 1, 1, 1, 'END OF STOCK FOR White', 1, 1, 1, 1, 1, 'END OF STOCK FOR Black'</t>
+  </si>
+  <si>
+    <t>1, 1, 1, 1, 0, 'END OF STOCK FOR Red', 1, 1, 1, 1, 0, 'END OF STOCK FOR Black', 1, 1, 1, 1, 1, 'END OF STOCK FOR White'</t>
+  </si>
+  <si>
+    <t>0, 0, 0, 0, 0, 'END OF STOCK FOR Red', 1, 1, 1, 1, 1, 'END OF STOCK FOR White', 1, 1, 1, 1, 1, 'END OF STOCK FOR Black'</t>
+  </si>
+  <si>
+    <t>1, 'END OF STOCK FOR White', 1, 'END OF STOCK FOR Black'</t>
   </si>
 </sst>
 </file>
@@ -1505,13 +1715,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N71"/>
+  <dimension ref="A1:O71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1554,19 +1764,22 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2">
         <v>307053</v>
       </c>
       <c r="C2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E2">
         <v>138</v>
@@ -1587,30 +1800,33 @@
         <v>53</v>
       </c>
       <c r="K2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="L2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="M2" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="N2" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
+        <v>370</v>
+      </c>
+      <c r="O2" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B3">
         <v>307009</v>
       </c>
       <c r="C3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E3">
         <v>128</v>
@@ -1631,30 +1847,33 @@
         <v>54</v>
       </c>
       <c r="K3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="L3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="M3" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="N3" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
+        <v>370</v>
+      </c>
+      <c r="O3" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4">
         <v>307037</v>
       </c>
       <c r="C4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D4" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E4">
         <v>128</v>
@@ -1675,30 +1894,33 @@
         <v>55</v>
       </c>
       <c r="K4" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="L4" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="M4" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="N4" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
+        <v>370</v>
+      </c>
+      <c r="O4" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5">
         <v>307049</v>
       </c>
       <c r="C5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D5" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E5">
         <v>46</v>
@@ -1719,30 +1941,33 @@
         <v>56</v>
       </c>
       <c r="K5" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="L5" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="M5" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="N5" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
+        <v>370</v>
+      </c>
+      <c r="O5" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6">
         <v>307022</v>
       </c>
       <c r="C6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D6" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E6">
         <v>42</v>
@@ -1763,30 +1988,33 @@
         <v>57</v>
       </c>
       <c r="K6" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="L6" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="M6" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="N6" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
+        <v>370</v>
+      </c>
+      <c r="O6" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7">
         <v>307004</v>
       </c>
       <c r="C7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D7" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E7">
         <v>48</v>
@@ -1807,30 +2035,33 @@
         <v>58</v>
       </c>
       <c r="K7" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="L7" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="M7" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="N7" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
+        <v>370</v>
+      </c>
+      <c r="O7" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B8">
         <v>307023</v>
       </c>
       <c r="C8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D8" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E8">
         <v>64</v>
@@ -1851,30 +2082,33 @@
         <v>66</v>
       </c>
       <c r="K8" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="L8" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="M8" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="N8" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
+        <v>371</v>
+      </c>
+      <c r="O8" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B9">
         <v>307054</v>
       </c>
       <c r="C9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D9" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E9">
         <v>32</v>
@@ -1895,30 +2129,33 @@
         <v>67</v>
       </c>
       <c r="K9" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="L9" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="M9" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="N9" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
+        <v>372</v>
+      </c>
+      <c r="O9" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B10">
         <v>307011</v>
       </c>
       <c r="C10" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D10" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E10">
         <v>58</v>
@@ -1939,30 +2176,33 @@
         <v>68</v>
       </c>
       <c r="K10" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="L10" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="M10" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="N10" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
+        <v>373</v>
+      </c>
+      <c r="O10" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B11">
         <v>307039</v>
       </c>
       <c r="C11" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D11" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E11">
         <v>58</v>
@@ -1983,30 +2223,33 @@
         <v>69</v>
       </c>
       <c r="K11" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="L11" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="M11" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="N11" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
+        <v>374</v>
+      </c>
+      <c r="O11" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B12">
         <v>307085</v>
       </c>
       <c r="C12" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D12" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E12">
         <v>138</v>
@@ -2027,30 +2270,33 @@
         <v>13</v>
       </c>
       <c r="K12" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="L12" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="M12" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="N12" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
+        <v>375</v>
+      </c>
+      <c r="O12" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B13">
         <v>307070</v>
       </c>
       <c r="C13" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D13" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E13">
         <v>128</v>
@@ -2071,30 +2317,33 @@
         <v>14</v>
       </c>
       <c r="K13" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="L13" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="M13" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="N13" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14">
+        <v>375</v>
+      </c>
+      <c r="O13" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B14">
         <v>306984</v>
       </c>
       <c r="C14" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D14" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E14">
         <v>110</v>
@@ -2115,27 +2364,30 @@
         <v>15</v>
       </c>
       <c r="K14" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="M14" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="N14" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
+        <v>375</v>
+      </c>
+      <c r="O14" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B15">
         <v>307034</v>
       </c>
       <c r="C15" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D15" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E15">
         <v>110</v>
@@ -2156,30 +2408,33 @@
         <v>16</v>
       </c>
       <c r="K15" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="L15" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="M15" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="N15" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
+        <v>375</v>
+      </c>
+      <c r="O15" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B16">
         <v>307090</v>
       </c>
       <c r="C16" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D16" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E16">
         <v>178</v>
@@ -2200,30 +2455,33 @@
         <v>3</v>
       </c>
       <c r="K16" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="L16" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="M16" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="N16" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14">
+        <v>375</v>
+      </c>
+      <c r="O16" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B17">
         <v>307079</v>
       </c>
       <c r="C17" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D17" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E17">
         <v>128</v>
@@ -2244,30 +2502,33 @@
         <v>36</v>
       </c>
       <c r="K17" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="L17" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="M17" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="N17" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14">
+        <v>376</v>
+      </c>
+      <c r="O17" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B18">
         <v>307074</v>
       </c>
       <c r="C18" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D18" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E18">
         <v>158</v>
@@ -2288,30 +2549,33 @@
         <v>37</v>
       </c>
       <c r="K18" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="L18" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="M18" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="N18" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14">
+        <v>376</v>
+      </c>
+      <c r="O18" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B19">
         <v>307010</v>
       </c>
       <c r="C19" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D19" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E19">
         <v>158</v>
@@ -2332,30 +2596,33 @@
         <v>38</v>
       </c>
       <c r="K19" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="L19" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="M19" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="N19" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14">
+        <v>376</v>
+      </c>
+      <c r="O19" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B20">
         <v>307056</v>
       </c>
       <c r="C20" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D20" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E20">
         <v>118</v>
@@ -2376,30 +2643,33 @@
         <v>39</v>
       </c>
       <c r="K20" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="L20" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="M20" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="N20" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14">
+        <v>377</v>
+      </c>
+      <c r="O20" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B21">
         <v>307064</v>
       </c>
       <c r="C21" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D21" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E21">
         <v>148</v>
@@ -2420,30 +2690,33 @@
         <v>40</v>
       </c>
       <c r="K21" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="L21" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="M21" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="N21" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14">
+        <v>376</v>
+      </c>
+      <c r="O21" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B22">
         <v>307031</v>
       </c>
       <c r="C22" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D22" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E22">
         <v>158</v>
@@ -2464,30 +2737,33 @@
         <v>41</v>
       </c>
       <c r="K22" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="L22" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="M22" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="N22" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14">
+        <v>377</v>
+      </c>
+      <c r="O22" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B23">
         <v>307026</v>
       </c>
       <c r="C23" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D23" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E23">
         <v>148</v>
@@ -2508,30 +2784,33 @@
         <v>42</v>
       </c>
       <c r="K23" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="L23" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="M23" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="N23" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14">
+        <v>376</v>
+      </c>
+      <c r="O23" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B24">
         <v>307006</v>
       </c>
       <c r="C24" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D24" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E24">
         <v>158</v>
@@ -2552,30 +2831,33 @@
         <v>43</v>
       </c>
       <c r="K24" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="L24" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="M24" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="N24" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14">
+        <v>376</v>
+      </c>
+      <c r="O24" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
       <c r="A25" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B25">
         <v>307014</v>
       </c>
       <c r="C25" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D25" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E25">
         <v>168</v>
@@ -2596,30 +2878,33 @@
         <v>44</v>
       </c>
       <c r="K25" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="L25" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="M25" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="N25" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14">
+        <v>376</v>
+      </c>
+      <c r="O25" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B26">
         <v>306998</v>
       </c>
       <c r="C26" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D26" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E26">
         <v>148</v>
@@ -2640,30 +2925,33 @@
         <v>45</v>
       </c>
       <c r="K26" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="L26" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="M26" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="N26" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14">
+        <v>376</v>
+      </c>
+      <c r="O26" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B27">
         <v>307087</v>
       </c>
       <c r="C27" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D27" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E27">
         <v>118</v>
@@ -2684,30 +2972,33 @@
         <v>4</v>
       </c>
       <c r="K27" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="L27" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="M27" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="N27" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14">
+        <v>375</v>
+      </c>
+      <c r="O27" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
       <c r="A28" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B28">
         <v>307016</v>
       </c>
       <c r="C28" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D28" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E28">
         <v>110</v>
@@ -2728,30 +3019,33 @@
         <v>46</v>
       </c>
       <c r="K28" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="L28" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="M28" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="N28" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14">
+        <v>377</v>
+      </c>
+      <c r="O28" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
       <c r="A29" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B29">
         <v>307086</v>
       </c>
       <c r="C29" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D29" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E29">
         <v>98</v>
@@ -2772,30 +3066,33 @@
         <v>2</v>
       </c>
       <c r="K29" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L29" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="M29" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="N29" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14">
+        <v>375</v>
+      </c>
+      <c r="O29" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
       <c r="A30" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B30">
         <v>307082</v>
       </c>
       <c r="C30" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D30" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E30">
         <v>42</v>
@@ -2816,30 +3113,33 @@
         <v>6</v>
       </c>
       <c r="K30" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L30" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="M30" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="N30" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14">
+        <v>375</v>
+      </c>
+      <c r="O30" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
       <c r="A31" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B31">
         <v>307084</v>
       </c>
       <c r="C31" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D31" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E31">
         <v>138</v>
@@ -2860,30 +3160,33 @@
         <v>11</v>
       </c>
       <c r="K31" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L31" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="M31" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="N31" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14">
+        <v>375</v>
+      </c>
+      <c r="O31" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15">
       <c r="A32" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B32">
         <v>307092</v>
       </c>
       <c r="C32" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D32" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E32">
         <v>88</v>
@@ -2904,30 +3207,33 @@
         <v>24</v>
       </c>
       <c r="K32" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L32" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="M32" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="N32" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14">
+        <v>377</v>
+      </c>
+      <c r="O32" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
       <c r="A33" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B33">
         <v>307080</v>
       </c>
       <c r="C33" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D33" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E33">
         <v>78</v>
@@ -2948,30 +3254,33 @@
         <v>25</v>
       </c>
       <c r="K33" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L33" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="M33" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="N33" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14">
+        <v>377</v>
+      </c>
+      <c r="O33" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
       <c r="A34" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B34">
         <v>307018</v>
       </c>
       <c r="C34" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D34" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E34">
         <v>178</v>
@@ -2992,30 +3301,33 @@
         <v>12</v>
       </c>
       <c r="K34" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L34" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="M34" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="N34" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14">
+        <v>375</v>
+      </c>
+      <c r="O34" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
       <c r="A35" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B35">
         <v>307060</v>
       </c>
       <c r="C35" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D35" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E35">
         <v>118</v>
@@ -3036,30 +3348,33 @@
         <v>26</v>
       </c>
       <c r="K35" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L35" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="M35" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="N35" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14">
+        <v>377</v>
+      </c>
+      <c r="O35" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15">
       <c r="A36" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B36">
         <v>306999</v>
       </c>
       <c r="C36" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D36" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E36">
         <v>68</v>
@@ -3080,30 +3395,33 @@
         <v>27</v>
       </c>
       <c r="K36" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L36" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="M36" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="N36" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14">
+        <v>377</v>
+      </c>
+      <c r="O36" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
       <c r="A37" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B37">
         <v>307059</v>
       </c>
       <c r="C37" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D37" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E37">
         <v>88</v>
@@ -3124,30 +3442,33 @@
         <v>28</v>
       </c>
       <c r="K37" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L37" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="M37" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="N37" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14">
+        <v>377</v>
+      </c>
+      <c r="O37" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
       <c r="A38" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B38">
         <v>307015</v>
       </c>
       <c r="C38" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D38" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E38">
         <v>52</v>
@@ -3168,30 +3489,33 @@
         <v>29</v>
       </c>
       <c r="K38" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L38" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="M38" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="N38" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14">
+        <v>377</v>
+      </c>
+      <c r="O38" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15">
       <c r="A39" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B39">
         <v>307062</v>
       </c>
       <c r="C39" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D39" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E39">
         <v>78</v>
@@ -3212,30 +3536,33 @@
         <v>30</v>
       </c>
       <c r="K39" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L39" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="M39" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="N39" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14">
+        <v>377</v>
+      </c>
+      <c r="O39" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15">
       <c r="A40" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B40">
         <v>307051</v>
       </c>
       <c r="C40" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D40" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E40">
         <v>40</v>
@@ -3256,30 +3583,33 @@
         <v>31</v>
       </c>
       <c r="K40" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="L40" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="M40" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="N40" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14">
+        <v>377</v>
+      </c>
+      <c r="O40" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15">
       <c r="A41" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B41">
         <v>307050</v>
       </c>
       <c r="C41" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D41" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E41">
         <v>40</v>
@@ -3300,30 +3630,33 @@
         <v>32</v>
       </c>
       <c r="K41" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="L41" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="M41" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="N41" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14">
+        <v>377</v>
+      </c>
+      <c r="O41" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15">
       <c r="A42" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B42">
         <v>306985</v>
       </c>
       <c r="C42" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D42" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E42">
         <v>40</v>
@@ -3344,30 +3677,33 @@
         <v>33</v>
       </c>
       <c r="K42" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="L42" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="M42" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="N42" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14">
+        <v>377</v>
+      </c>
+      <c r="O42" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15">
       <c r="A43" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B43">
         <v>306996</v>
       </c>
       <c r="C43" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D43" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E43">
         <v>40</v>
@@ -3388,30 +3724,33 @@
         <v>34</v>
       </c>
       <c r="K43" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="L43" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="M43" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="N43" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14">
+        <v>377</v>
+      </c>
+      <c r="O43" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15">
       <c r="A44" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B44">
         <v>307044</v>
       </c>
       <c r="C44" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D44" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E44">
         <v>40</v>
@@ -3432,30 +3771,33 @@
         <v>35</v>
       </c>
       <c r="K44" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="L44" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="M44" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="N44" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14">
+        <v>377</v>
+      </c>
+      <c r="O44" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15">
       <c r="A45" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B45">
         <v>307081</v>
       </c>
       <c r="C45" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D45" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E45">
         <v>288</v>
@@ -3476,30 +3818,33 @@
         <v>0</v>
       </c>
       <c r="K45" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="L45" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="M45" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="N45" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14">
+        <v>375</v>
+      </c>
+      <c r="O45" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15">
       <c r="A46" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B46">
         <v>307076</v>
       </c>
       <c r="C46" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D46" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E46">
         <v>208</v>
@@ -3520,30 +3865,33 @@
         <v>1</v>
       </c>
       <c r="K46" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="L46" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="M46" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="N46" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14">
+        <v>375</v>
+      </c>
+      <c r="O46" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15">
       <c r="A47" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B47">
         <v>307042</v>
       </c>
       <c r="C47" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D47" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E47">
         <v>178</v>
@@ -3564,30 +3912,33 @@
         <v>7</v>
       </c>
       <c r="K47" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="L47" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="M47" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="N47" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14">
+        <v>377</v>
+      </c>
+      <c r="O47" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15">
       <c r="A48" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B48">
         <v>307068</v>
       </c>
       <c r="C48" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D48" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E48">
         <v>178</v>
@@ -3608,30 +3959,33 @@
         <v>8</v>
       </c>
       <c r="K48" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="L48" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="M48" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="N48" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14">
+        <v>375</v>
+      </c>
+      <c r="O48" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15">
       <c r="A49" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B49">
         <v>306997</v>
       </c>
       <c r="C49" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D49" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E49">
         <v>428</v>
@@ -3652,30 +4006,33 @@
         <v>9</v>
       </c>
       <c r="K49" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="L49" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="M49" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="N49" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14">
+        <v>375</v>
+      </c>
+      <c r="O49" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15">
       <c r="A50" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B50">
         <v>307067</v>
       </c>
       <c r="C50" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D50" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E50">
         <v>128</v>
@@ -3696,30 +4053,33 @@
         <v>10</v>
       </c>
       <c r="K50" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="L50" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="M50" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="N50" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14">
+        <v>377</v>
+      </c>
+      <c r="O50" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15">
       <c r="A51" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B51">
         <v>307077</v>
       </c>
       <c r="C51" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D51" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E51">
         <v>178</v>
@@ -3740,30 +4100,33 @@
         <v>17</v>
       </c>
       <c r="K51" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="L51" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="M51" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="N51" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14">
+        <v>377</v>
+      </c>
+      <c r="O51" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15">
       <c r="A52" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B52">
         <v>307078</v>
       </c>
       <c r="C52" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D52" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E52">
         <v>148</v>
@@ -3784,30 +4147,33 @@
         <v>18</v>
       </c>
       <c r="K52" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="L52" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="M52" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="N52" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14">
+        <v>377</v>
+      </c>
+      <c r="O52" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15">
       <c r="A53" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B53">
         <v>306989</v>
       </c>
       <c r="C53" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D53" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E53">
         <v>168</v>
@@ -3828,30 +4194,33 @@
         <v>19</v>
       </c>
       <c r="K53" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="L53" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="M53" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="N53" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14">
+        <v>377</v>
+      </c>
+      <c r="O53" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15">
       <c r="A54" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B54">
         <v>307073</v>
       </c>
       <c r="C54" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D54" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E54">
         <v>148</v>
@@ -3872,30 +4241,33 @@
         <v>20</v>
       </c>
       <c r="K54" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="L54" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="M54" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="N54" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14">
+        <v>377</v>
+      </c>
+      <c r="O54" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15">
       <c r="A55" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B55">
         <v>307030</v>
       </c>
       <c r="C55" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D55" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E55">
         <v>128</v>
@@ -3916,30 +4288,33 @@
         <v>21</v>
       </c>
       <c r="K55" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="L55" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="M55" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="N55" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14">
+        <v>377</v>
+      </c>
+      <c r="O55" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15">
       <c r="A56" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B56">
         <v>307005</v>
       </c>
       <c r="C56" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D56" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E56">
         <v>148</v>
@@ -3960,30 +4335,33 @@
         <v>22</v>
       </c>
       <c r="K56" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="L56" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="M56" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="N56" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14">
+        <v>377</v>
+      </c>
+      <c r="O56" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15">
       <c r="A57" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B57">
         <v>307071</v>
       </c>
       <c r="C57" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D57" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E57">
         <v>168</v>
@@ -4004,30 +4382,33 @@
         <v>23</v>
       </c>
       <c r="K57" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="L57" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="M57" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="N57" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14">
+        <v>377</v>
+      </c>
+      <c r="O57" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15">
       <c r="A58" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B58">
         <v>307083</v>
       </c>
       <c r="C58" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D58" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E58">
         <v>42</v>
@@ -4048,30 +4429,33 @@
         <v>5</v>
       </c>
       <c r="K58" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L58" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="M58" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="N58" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14">
+        <v>370</v>
+      </c>
+      <c r="O58" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15">
       <c r="A59" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B59">
         <v>307089</v>
       </c>
       <c r="C59" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D59" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E59">
         <v>46</v>
@@ -4092,30 +4476,33 @@
         <v>47</v>
       </c>
       <c r="K59" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L59" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="M59" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="N59" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="60" spans="1:14">
+        <v>370</v>
+      </c>
+      <c r="O59" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15">
       <c r="A60" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B60">
         <v>307088</v>
       </c>
       <c r="C60" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D60" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E60">
         <v>50</v>
@@ -4136,30 +4523,33 @@
         <v>48</v>
       </c>
       <c r="K60" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L60" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="M60" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="N60" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14">
+        <v>370</v>
+      </c>
+      <c r="O60" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15">
       <c r="A61" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B61">
         <v>307000</v>
       </c>
       <c r="C61" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D61" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E61">
         <v>46</v>
@@ -4180,30 +4570,33 @@
         <v>49</v>
       </c>
       <c r="K61" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L61" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="M61" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="N61" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14">
+        <v>370</v>
+      </c>
+      <c r="O61" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15">
       <c r="A62" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B62">
         <v>307075</v>
       </c>
       <c r="C62" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D62" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E62">
         <v>54</v>
@@ -4224,30 +4617,33 @@
         <v>50</v>
       </c>
       <c r="K62" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L62" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="M62" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="N62" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="63" spans="1:14">
+        <v>378</v>
+      </c>
+      <c r="O62" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15">
       <c r="A63" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B63">
         <v>306986</v>
       </c>
       <c r="C63" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D63" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E63">
         <v>44</v>
@@ -4268,30 +4664,33 @@
         <v>51</v>
       </c>
       <c r="K63" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L63" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="M63" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="N63" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="64" spans="1:14">
+        <v>370</v>
+      </c>
+      <c r="O63" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15">
       <c r="A64" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B64">
         <v>306981</v>
       </c>
       <c r="C64" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D64" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E64">
         <v>34</v>
@@ -4312,30 +4711,33 @@
         <v>52</v>
       </c>
       <c r="K64" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L64" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="M64" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="N64" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="65" spans="1:14">
+        <v>370</v>
+      </c>
+      <c r="O64" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15">
       <c r="A65" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B65">
         <v>307091</v>
       </c>
       <c r="C65" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D65" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E65">
         <v>88</v>
@@ -4356,30 +4758,33 @@
         <v>59</v>
       </c>
       <c r="K65" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="L65" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="M65" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="N65" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="66" spans="1:14">
+        <v>370</v>
+      </c>
+      <c r="O65" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15">
       <c r="A66" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B66">
         <v>307002</v>
       </c>
       <c r="C66" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D66" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E66">
         <v>48</v>
@@ -4400,30 +4805,33 @@
         <v>60</v>
       </c>
       <c r="K66" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="L66" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="M66" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="N66" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="67" spans="1:14">
+        <v>370</v>
+      </c>
+      <c r="O66" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15">
       <c r="A67" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B67">
         <v>307007</v>
       </c>
       <c r="C67" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D67" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E67">
         <v>28</v>
@@ -4444,30 +4852,33 @@
         <v>61</v>
       </c>
       <c r="K67" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="L67" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="M67" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="N67" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="68" spans="1:14">
+        <v>377</v>
+      </c>
+      <c r="O67" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15">
       <c r="A68" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B68">
         <v>306994</v>
       </c>
       <c r="C68" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D68" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E68">
         <v>30</v>
@@ -4488,30 +4899,33 @@
         <v>62</v>
       </c>
       <c r="K68" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="L68" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="M68" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="N68" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="69" spans="1:14">
+        <v>377</v>
+      </c>
+      <c r="O68" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15">
       <c r="A69" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B69">
         <v>307041</v>
       </c>
       <c r="C69" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D69" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E69">
         <v>36</v>
@@ -4532,30 +4946,33 @@
         <v>63</v>
       </c>
       <c r="K69" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="L69" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="M69" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="N69" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="70" spans="1:14">
+        <v>377</v>
+      </c>
+      <c r="O69" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15">
       <c r="A70" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B70">
         <v>307043</v>
       </c>
       <c r="C70" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D70" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E70">
         <v>28</v>
@@ -4576,30 +4993,33 @@
         <v>64</v>
       </c>
       <c r="K70" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="L70" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="M70" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="N70" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="71" spans="1:14">
+        <v>377</v>
+      </c>
+      <c r="O70" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15">
       <c r="A71" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B71">
         <v>307046</v>
       </c>
       <c r="C71" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D71" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E71">
         <v>20</v>
@@ -4620,16 +5040,19 @@
         <v>65</v>
       </c>
       <c r="K71" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="L71" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="M71" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="N71" t="s">
-        <v>369</v>
+        <v>370</v>
+      </c>
+      <c r="O71" t="s">
+        <v>447</v>
       </c>
     </row>
   </sheetData>

</xml_diff>